<commit_message>
artworks detail page thumbnail z-index fixed
</commit_message>
<xml_diff>
--- a/Artworks.xlsx
+++ b/Artworks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangjin/web_renewal/hijonam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77DFA457-1DE3-EC46-AF4B-E8F87FDB951B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0C4F275-50DE-EE43-8811-B043CD6D12CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11160" yWindow="3520" windowWidth="25640" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1060" yWindow="8400" windowWidth="25640" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="744" uniqueCount="325">
   <si>
     <t>category</t>
   </si>
@@ -987,6 +987,18 @@
   </si>
   <si>
     <t>A Bulging Image-0.jpg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ottchil (Korean Lacquer Work)</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Installation</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Fabric Collage</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1377,8 +1389,8 @@
   <dimension ref="A1:I148"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I4" sqref="I4"/>
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
@@ -1689,7 +1701,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>324</v>
       </c>
       <c r="C11" t="s">
         <v>31</v>
@@ -2936,7 +2948,7 @@
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>118</v>
+        <v>322</v>
       </c>
       <c r="C54" t="s">
         <v>119</v>
@@ -4212,7 +4224,7 @@
         <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>209</v>
+        <v>323</v>
       </c>
       <c r="C98" t="s">
         <v>210</v>

</xml_diff>

<commit_message>
Time Period -> Work Year // Font size fixed
</commit_message>
<xml_diff>
--- a/Artworks.xlsx
+++ b/Artworks.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sangjin/web_renewal/hijonam/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66E570F8-A575-6F40-BA67-316193D3BA0D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E837375-A13B-134C-839C-F3294717F3DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="18960" yWindow="4720" windowWidth="29020" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="6980" yWindow="4720" windowWidth="29020" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="248">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="676" uniqueCount="247">
   <si>
     <t>category</t>
   </si>
@@ -185,9 +185,6 @@
     <t>Spring Sonata 3</t>
   </si>
   <si>
-    <t>Ottchil (Korean Lacquer Work)</t>
-  </si>
-  <si>
     <t>Liberal Ashanti1_1</t>
   </si>
   <si>
@@ -465,10 +462,6 @@
   </si>
   <si>
     <t>The Masks</t>
-  </si>
-  <si>
-    <t>Ottchil (Korean Lacquer Work)</t>
-    <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
     <t>Installation</t>
@@ -820,6 +813,10 @@
   </si>
   <si>
     <t>Journey 5 Fabric collage on Canvas 53x72.2cm_2022.jpg</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ottchil</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -1218,14 +1215,14 @@
   <dimension ref="A1:J128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E115" sqref="E115"/>
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B55" sqref="B55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="17"/>
   <cols>
     <col min="1" max="1" width="2.83203125" customWidth="1"/>
-    <col min="2" max="2" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="30.83203125" customWidth="1"/>
     <col min="3" max="3" width="29.33203125" customWidth="1"/>
     <col min="4" max="4" width="12.5" style="4" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="29.1640625" bestFit="1" customWidth="1"/>
@@ -1265,7 +1262,7 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -1282,7 +1279,7 @@
         <v>0</v>
       </c>
       <c r="E2" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="F2" s="7">
         <v>72.7</v>
@@ -1294,13 +1291,13 @@
         <v>2022</v>
       </c>
       <c r="I2" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="J2" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="19.5" customHeight="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -1308,7 +1305,7 @@
         <v>12</v>
       </c>
       <c r="C3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D3" s="3">
         <v>1</v>
@@ -1326,13 +1323,13 @@
         <v>2012</v>
       </c>
       <c r="I3" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J3" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -1340,13 +1337,13 @@
         <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D4" s="3">
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F4" s="7">
         <v>69.400000000000006</v>
@@ -1358,13 +1355,13 @@
         <v>2017</v>
       </c>
       <c r="I4" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="J4" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -1372,13 +1369,13 @@
         <v>12</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D5" s="3">
         <v>3</v>
       </c>
       <c r="E5" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="F5" s="7">
         <v>50</v>
@@ -1390,13 +1387,13 @@
         <v>2017</v>
       </c>
       <c r="I5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J5" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -1404,13 +1401,13 @@
         <v>12</v>
       </c>
       <c r="C6" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D6" s="3">
         <v>7</v>
       </c>
       <c r="E6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F6" s="7">
         <v>50</v>
@@ -1422,13 +1419,13 @@
         <v>2013</v>
       </c>
       <c r="I6" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="J6" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -1436,13 +1433,13 @@
         <v>12</v>
       </c>
       <c r="C7" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D7" s="3">
         <v>8</v>
       </c>
       <c r="E7" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="F7" s="7">
         <v>50</v>
@@ -1454,13 +1451,13 @@
         <v>2013</v>
       </c>
       <c r="I7" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="J7" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -1468,7 +1465,7 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D8" s="3">
         <v>17</v>
@@ -1486,13 +1483,13 @@
         <v>2015</v>
       </c>
       <c r="I8" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="J8" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -1500,7 +1497,7 @@
         <v>12</v>
       </c>
       <c r="C9" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D9" s="3">
         <v>18</v>
@@ -1518,13 +1515,13 @@
         <v>2022</v>
       </c>
       <c r="I9" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="J9" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -1532,7 +1529,7 @@
         <v>12</v>
       </c>
       <c r="C10" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D10" s="3">
         <v>19</v>
@@ -1550,13 +1547,13 @@
         <v>2022</v>
       </c>
       <c r="I10" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="J10" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1564,13 +1561,13 @@
         <v>12</v>
       </c>
       <c r="C11" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D11" s="3">
         <v>5</v>
       </c>
       <c r="E11" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F11" s="7">
         <v>50</v>
@@ -1582,13 +1579,13 @@
         <v>2017</v>
       </c>
       <c r="I11" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="J11" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A12" t="s">
         <v>9</v>
       </c>
@@ -1596,7 +1593,7 @@
         <v>12</v>
       </c>
       <c r="C12" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D12" s="3">
         <v>20</v>
@@ -1614,13 +1611,13 @@
         <v>2022</v>
       </c>
       <c r="I12" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J12" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -1628,7 +1625,7 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D13" s="3">
         <v>21</v>
@@ -1646,13 +1643,13 @@
         <v>2022</v>
       </c>
       <c r="I13" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="J13" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -1660,13 +1657,13 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D14" s="3">
         <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="F14" s="7">
         <v>63.5</v>
@@ -1678,10 +1675,10 @@
         <v>2012</v>
       </c>
       <c r="I14" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="J14" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="15" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -1689,7 +1686,7 @@
         <v>9</v>
       </c>
       <c r="B15" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="C15" t="s">
         <v>16</v>
@@ -1710,10 +1707,10 @@
         <v>2022</v>
       </c>
       <c r="I15" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J15" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="16" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -1742,10 +1739,10 @@
         <v>2022</v>
       </c>
       <c r="I16" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="J16" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="17" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -1774,10 +1771,10 @@
         <v>2022</v>
       </c>
       <c r="I17" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="J17" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -1806,10 +1803,10 @@
         <v>2022</v>
       </c>
       <c r="I18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="J18" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="19" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -1838,10 +1835,10 @@
         <v>2022</v>
       </c>
       <c r="I19" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="J19" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -1870,10 +1867,10 @@
         <v>2022</v>
       </c>
       <c r="I20" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="J20" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
     </row>
     <row r="21" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -1902,13 +1899,13 @@
         <v>2022</v>
       </c>
       <c r="I21" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="J21" t="s">
-        <v>247</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="19.5" customHeight="1">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1916,7 +1913,7 @@
         <v>12</v>
       </c>
       <c r="C22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="D22" s="3">
         <v>6</v>
@@ -1934,13 +1931,13 @@
         <v>2015</v>
       </c>
       <c r="I22" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="J22" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -1948,13 +1945,13 @@
         <v>12</v>
       </c>
       <c r="C23" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D23" s="3">
         <v>103</v>
       </c>
       <c r="E23" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="F23" s="7">
         <v>50</v>
@@ -1966,13 +1963,13 @@
         <v>2014</v>
       </c>
       <c r="I23" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="J23" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1980,13 +1977,13 @@
         <v>12</v>
       </c>
       <c r="C24" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D24" s="3">
         <v>104</v>
       </c>
       <c r="E24" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F24" s="7">
         <v>50</v>
@@ -1998,13 +1995,13 @@
         <v>2014</v>
       </c>
       <c r="I24" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="J24" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -2012,13 +2009,13 @@
         <v>12</v>
       </c>
       <c r="C25" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D25" s="3">
         <v>22</v>
       </c>
       <c r="E25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F25" s="7">
         <v>50</v>
@@ -2030,13 +2027,13 @@
         <v>2017</v>
       </c>
       <c r="I25" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="J25" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="19.5" customHeight="1">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" ht="19.5" hidden="1" customHeight="1">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -2044,13 +2041,13 @@
         <v>12</v>
       </c>
       <c r="C26" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="D26" s="3">
         <v>23</v>
       </c>
       <c r="E26" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="F26" s="7">
         <v>50</v>
@@ -2062,10 +2059,10 @@
         <v>2017</v>
       </c>
       <c r="I26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="J26" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
     </row>
     <row r="27" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2094,10 +2091,10 @@
         <v>2022</v>
       </c>
       <c r="I27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="J27" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="28" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2126,10 +2123,10 @@
         <v>2018</v>
       </c>
       <c r="I28" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="J28" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="29" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2158,10 +2155,10 @@
         <v>2022</v>
       </c>
       <c r="I29" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="J29" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="30" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2190,10 +2187,10 @@
         <v>2022</v>
       </c>
       <c r="I30" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="J30" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2222,10 +2219,10 @@
         <v>2022</v>
       </c>
       <c r="I31" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="J31" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="32" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2254,10 +2251,10 @@
         <v>2022</v>
       </c>
       <c r="I32" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="J32" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="33" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2286,10 +2283,10 @@
         <v>2018</v>
       </c>
       <c r="I33" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="J33" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="34" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2318,10 +2315,10 @@
         <v>2021</v>
       </c>
       <c r="I34" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="J34" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="35" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2350,10 +2347,10 @@
         <v>2021</v>
       </c>
       <c r="I35" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="J35" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2382,10 +2379,10 @@
         <v>2022</v>
       </c>
       <c r="I36" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="J36" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="37" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2414,10 +2411,10 @@
         <v>2022</v>
       </c>
       <c r="I37" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="J37" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="38" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2446,10 +2443,10 @@
         <v>2022</v>
       </c>
       <c r="I38" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="J38" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="39" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2478,10 +2475,10 @@
         <v>2022</v>
       </c>
       <c r="I39" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="J39" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="40" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2510,10 +2507,10 @@
         <v>2019</v>
       </c>
       <c r="I40" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="J40" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="41" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2542,10 +2539,10 @@
         <v>2019</v>
       </c>
       <c r="I41" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="J41" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="42" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2574,10 +2571,10 @@
         <v>2022</v>
       </c>
       <c r="I42" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="J42" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="43" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2606,10 +2603,10 @@
         <v>2022</v>
       </c>
       <c r="I43" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="J43" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="44" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2638,10 +2635,10 @@
         <v>2022</v>
       </c>
       <c r="I44" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="J44" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="45" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2670,10 +2667,10 @@
         <v>2022</v>
       </c>
       <c r="I45" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="J45" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="46" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -2702,1418 +2699,1418 @@
         <v>2022</v>
       </c>
       <c r="I46" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="J46" t="s">
-        <v>223</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" ht="19.5" customHeight="1">
       <c r="A47" t="s">
         <v>9</v>
       </c>
       <c r="B47" t="s">
-        <v>143</v>
+        <v>246</v>
       </c>
       <c r="C47" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D47" s="3">
         <v>44</v>
       </c>
       <c r="E47" t="s">
+        <v>49</v>
+      </c>
+      <c r="F47" s="7">
+        <v>0</v>
+      </c>
+      <c r="G47" s="7">
+        <v>0</v>
+      </c>
+      <c r="H47" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I47" t="s">
         <v>50</v>
       </c>
-      <c r="F47" s="7">
-        <v>0</v>
-      </c>
-      <c r="G47" s="7">
-        <v>0</v>
-      </c>
-      <c r="H47" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I47" t="s">
-        <v>51</v>
-      </c>
       <c r="J47" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" ht="19.5" customHeight="1">
       <c r="A48" t="s">
         <v>9</v>
       </c>
       <c r="B48" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C48" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D48" s="3">
         <v>45</v>
       </c>
       <c r="E48" t="s">
+        <v>51</v>
+      </c>
+      <c r="F48" s="7">
+        <v>0</v>
+      </c>
+      <c r="G48" s="7">
+        <v>0</v>
+      </c>
+      <c r="H48" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I48" t="s">
         <v>52</v>
       </c>
-      <c r="F48" s="7">
-        <v>0</v>
-      </c>
-      <c r="G48" s="7">
-        <v>0</v>
-      </c>
-      <c r="H48" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I48" t="s">
-        <v>53</v>
-      </c>
       <c r="J48" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" ht="19.5" customHeight="1">
       <c r="A49" t="s">
         <v>9</v>
       </c>
       <c r="B49" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C49" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D49" s="3">
         <v>46</v>
       </c>
       <c r="E49" t="s">
+        <v>53</v>
+      </c>
+      <c r="F49" s="7">
+        <v>0</v>
+      </c>
+      <c r="G49" s="7">
+        <v>0</v>
+      </c>
+      <c r="H49" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I49" t="s">
         <v>54</v>
       </c>
-      <c r="F49" s="7">
-        <v>0</v>
-      </c>
-      <c r="G49" s="7">
-        <v>0</v>
-      </c>
-      <c r="H49" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I49" t="s">
-        <v>55</v>
-      </c>
       <c r="J49" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" ht="19.5" customHeight="1">
       <c r="A50" t="s">
         <v>9</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C50" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D50" s="3">
         <v>47</v>
       </c>
       <c r="E50" t="s">
+        <v>55</v>
+      </c>
+      <c r="F50" s="7">
+        <v>0</v>
+      </c>
+      <c r="G50" s="7">
+        <v>0</v>
+      </c>
+      <c r="H50" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I50" t="s">
         <v>56</v>
       </c>
-      <c r="F50" s="7">
-        <v>0</v>
-      </c>
-      <c r="G50" s="7">
-        <v>0</v>
-      </c>
-      <c r="H50" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I50" t="s">
-        <v>57</v>
-      </c>
       <c r="J50" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" ht="19.5" customHeight="1">
       <c r="A51" t="s">
         <v>9</v>
       </c>
       <c r="B51" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C51" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D51" s="3">
         <v>48</v>
       </c>
       <c r="E51" t="s">
+        <v>57</v>
+      </c>
+      <c r="F51" s="7">
+        <v>0</v>
+      </c>
+      <c r="G51" s="7">
+        <v>0</v>
+      </c>
+      <c r="H51" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I51" t="s">
         <v>58</v>
       </c>
-      <c r="F51" s="7">
-        <v>0</v>
-      </c>
-      <c r="G51" s="7">
-        <v>0</v>
-      </c>
-      <c r="H51" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I51" t="s">
-        <v>59</v>
-      </c>
       <c r="J51" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" ht="19.5" customHeight="1">
       <c r="A52" t="s">
         <v>9</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C52" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D52" s="3">
         <v>49</v>
       </c>
       <c r="E52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F52" s="7">
+        <v>0</v>
+      </c>
+      <c r="G52" s="7">
+        <v>0</v>
+      </c>
+      <c r="H52" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I52" t="s">
         <v>60</v>
       </c>
-      <c r="F52" s="7">
-        <v>0</v>
-      </c>
-      <c r="G52" s="7">
-        <v>0</v>
-      </c>
-      <c r="H52" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I52" t="s">
-        <v>61</v>
-      </c>
       <c r="J52" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="53" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" ht="19.5" customHeight="1">
       <c r="A53" t="s">
         <v>9</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C53" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D53" s="3">
         <v>50</v>
       </c>
       <c r="E53" t="s">
+        <v>61</v>
+      </c>
+      <c r="F53" s="7">
+        <v>0</v>
+      </c>
+      <c r="G53" s="7">
+        <v>0</v>
+      </c>
+      <c r="H53" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I53" t="s">
         <v>62</v>
       </c>
-      <c r="F53" s="7">
-        <v>0</v>
-      </c>
-      <c r="G53" s="7">
-        <v>0</v>
-      </c>
-      <c r="H53" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I53" t="s">
-        <v>63</v>
-      </c>
       <c r="J53" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="54" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" ht="19.5" customHeight="1">
       <c r="A54" t="s">
         <v>9</v>
       </c>
       <c r="B54" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C54" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D54" s="3">
         <v>51</v>
       </c>
       <c r="E54" t="s">
+        <v>63</v>
+      </c>
+      <c r="F54" s="7">
+        <v>0</v>
+      </c>
+      <c r="G54" s="7">
+        <v>0</v>
+      </c>
+      <c r="H54" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I54" t="s">
         <v>64</v>
       </c>
-      <c r="F54" s="7">
-        <v>0</v>
-      </c>
-      <c r="G54" s="7">
-        <v>0</v>
-      </c>
-      <c r="H54" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I54" t="s">
-        <v>65</v>
-      </c>
       <c r="J54" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="55" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" ht="19.5" customHeight="1">
       <c r="A55" t="s">
         <v>9</v>
       </c>
       <c r="B55" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C55" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D55" s="3">
         <v>52</v>
       </c>
       <c r="E55" t="s">
+        <v>65</v>
+      </c>
+      <c r="F55" s="7">
+        <v>0</v>
+      </c>
+      <c r="G55" s="7">
+        <v>0</v>
+      </c>
+      <c r="H55" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I55" t="s">
         <v>66</v>
       </c>
-      <c r="F55" s="7">
-        <v>0</v>
-      </c>
-      <c r="G55" s="7">
-        <v>0</v>
-      </c>
-      <c r="H55" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I55" t="s">
-        <v>67</v>
-      </c>
       <c r="J55" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" ht="19.5" customHeight="1">
       <c r="A56" t="s">
         <v>9</v>
       </c>
       <c r="B56" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C56" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D56" s="3">
         <v>53</v>
       </c>
       <c r="E56" t="s">
+        <v>67</v>
+      </c>
+      <c r="F56" s="7">
+        <v>0</v>
+      </c>
+      <c r="G56" s="7">
+        <v>0</v>
+      </c>
+      <c r="H56" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I56" t="s">
         <v>68</v>
       </c>
-      <c r="F56" s="7">
-        <v>0</v>
-      </c>
-      <c r="G56" s="7">
-        <v>0</v>
-      </c>
-      <c r="H56" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I56" t="s">
-        <v>69</v>
-      </c>
       <c r="J56" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="57" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" ht="19.5" customHeight="1">
       <c r="A57" t="s">
         <v>9</v>
       </c>
       <c r="B57" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C57" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D57" s="3">
         <v>54</v>
       </c>
       <c r="E57" t="s">
+        <v>69</v>
+      </c>
+      <c r="F57" s="7">
+        <v>0</v>
+      </c>
+      <c r="G57" s="7">
+        <v>0</v>
+      </c>
+      <c r="H57" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I57" t="s">
         <v>70</v>
       </c>
-      <c r="F57" s="7">
-        <v>0</v>
-      </c>
-      <c r="G57" s="7">
-        <v>0</v>
-      </c>
-      <c r="H57" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I57" t="s">
-        <v>71</v>
-      </c>
       <c r="J57" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="58" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10" ht="19.5" customHeight="1">
       <c r="A58" t="s">
         <v>9</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C58" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D58" s="3">
         <v>55</v>
       </c>
       <c r="E58" t="s">
+        <v>71</v>
+      </c>
+      <c r="F58" s="7">
+        <v>0</v>
+      </c>
+      <c r="G58" s="7">
+        <v>0</v>
+      </c>
+      <c r="H58" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I58" t="s">
         <v>72</v>
       </c>
-      <c r="F58" s="7">
-        <v>0</v>
-      </c>
-      <c r="G58" s="7">
-        <v>0</v>
-      </c>
-      <c r="H58" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I58" t="s">
-        <v>73</v>
-      </c>
       <c r="J58" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="59" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" ht="19.5" customHeight="1">
       <c r="A59" t="s">
         <v>9</v>
       </c>
       <c r="B59" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C59" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D59" s="3">
         <v>56</v>
       </c>
       <c r="E59" t="s">
+        <v>73</v>
+      </c>
+      <c r="F59" s="7">
+        <v>0</v>
+      </c>
+      <c r="G59" s="7">
+        <v>0</v>
+      </c>
+      <c r="H59" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I59" t="s">
         <v>74</v>
       </c>
-      <c r="F59" s="7">
-        <v>0</v>
-      </c>
-      <c r="G59" s="7">
-        <v>0</v>
-      </c>
-      <c r="H59" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I59" t="s">
-        <v>75</v>
-      </c>
       <c r="J59" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="60" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" ht="19.5" customHeight="1">
       <c r="A60" t="s">
         <v>9</v>
       </c>
       <c r="B60" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C60" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D60" s="3">
         <v>57</v>
       </c>
       <c r="E60" t="s">
+        <v>75</v>
+      </c>
+      <c r="F60" s="7">
+        <v>0</v>
+      </c>
+      <c r="G60" s="7">
+        <v>0</v>
+      </c>
+      <c r="H60" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I60" t="s">
         <v>76</v>
       </c>
-      <c r="F60" s="7">
-        <v>0</v>
-      </c>
-      <c r="G60" s="7">
-        <v>0</v>
-      </c>
-      <c r="H60" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I60" t="s">
-        <v>77</v>
-      </c>
       <c r="J60" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="61" spans="1:10" ht="19.5" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" ht="19.5" customHeight="1">
       <c r="A61" t="s">
         <v>9</v>
       </c>
       <c r="B61" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C61" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D61" s="3">
         <v>58</v>
       </c>
       <c r="E61" t="s">
+        <v>77</v>
+      </c>
+      <c r="F61" s="7">
+        <v>0</v>
+      </c>
+      <c r="G61" s="7">
+        <v>0</v>
+      </c>
+      <c r="H61" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I61" t="s">
         <v>78</v>
       </c>
-      <c r="F61" s="7">
-        <v>0</v>
-      </c>
-      <c r="G61" s="7">
-        <v>0</v>
-      </c>
-      <c r="H61" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I61" t="s">
-        <v>79</v>
-      </c>
       <c r="J61" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="62" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" ht="17.25" customHeight="1">
       <c r="A62" t="s">
         <v>9</v>
       </c>
       <c r="B62" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C62" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D62" s="3">
         <v>59</v>
       </c>
       <c r="E62" t="s">
+        <v>79</v>
+      </c>
+      <c r="F62" s="7">
+        <v>0</v>
+      </c>
+      <c r="G62" s="7">
+        <v>0</v>
+      </c>
+      <c r="H62" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I62" t="s">
         <v>80</v>
       </c>
-      <c r="F62" s="7">
-        <v>0</v>
-      </c>
-      <c r="G62" s="7">
-        <v>0</v>
-      </c>
-      <c r="H62" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I62" t="s">
-        <v>81</v>
-      </c>
       <c r="J62" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="63" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" ht="17.25" customHeight="1">
       <c r="A63" t="s">
         <v>9</v>
       </c>
       <c r="B63" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C63" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D63" s="3">
         <v>60</v>
       </c>
       <c r="E63" t="s">
+        <v>81</v>
+      </c>
+      <c r="F63" s="7">
+        <v>0</v>
+      </c>
+      <c r="G63" s="7">
+        <v>0</v>
+      </c>
+      <c r="H63" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I63" t="s">
         <v>82</v>
       </c>
-      <c r="F63" s="7">
-        <v>0</v>
-      </c>
-      <c r="G63" s="7">
-        <v>0</v>
-      </c>
-      <c r="H63" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I63" t="s">
-        <v>83</v>
-      </c>
       <c r="J63" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="64" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" ht="17.25" customHeight="1">
       <c r="A64" t="s">
         <v>9</v>
       </c>
       <c r="B64" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C64" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D64" s="3">
         <v>61</v>
       </c>
       <c r="E64" t="s">
+        <v>83</v>
+      </c>
+      <c r="F64" s="7">
+        <v>0</v>
+      </c>
+      <c r="G64" s="7">
+        <v>0</v>
+      </c>
+      <c r="H64" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I64" t="s">
         <v>84</v>
       </c>
-      <c r="F64" s="7">
-        <v>0</v>
-      </c>
-      <c r="G64" s="7">
-        <v>0</v>
-      </c>
-      <c r="H64" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I64" t="s">
-        <v>85</v>
-      </c>
       <c r="J64" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="65" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10" ht="17.25" customHeight="1">
       <c r="A65" t="s">
         <v>9</v>
       </c>
       <c r="B65" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C65" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D65" s="3">
         <v>62</v>
       </c>
       <c r="E65" t="s">
+        <v>85</v>
+      </c>
+      <c r="F65" s="7">
+        <v>0</v>
+      </c>
+      <c r="G65" s="7">
+        <v>0</v>
+      </c>
+      <c r="H65" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I65" t="s">
         <v>86</v>
       </c>
-      <c r="F65" s="7">
-        <v>0</v>
-      </c>
-      <c r="G65" s="7">
-        <v>0</v>
-      </c>
-      <c r="H65" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I65" t="s">
-        <v>87</v>
-      </c>
       <c r="J65" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="66" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" ht="17.25" customHeight="1">
       <c r="A66" t="s">
         <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C66" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D66" s="3">
         <v>63</v>
       </c>
       <c r="E66" t="s">
+        <v>87</v>
+      </c>
+      <c r="F66" s="7">
+        <v>0</v>
+      </c>
+      <c r="G66" s="7">
+        <v>0</v>
+      </c>
+      <c r="H66" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I66" t="s">
         <v>88</v>
       </c>
-      <c r="F66" s="7">
-        <v>0</v>
-      </c>
-      <c r="G66" s="7">
-        <v>0</v>
-      </c>
-      <c r="H66" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I66" t="s">
-        <v>89</v>
-      </c>
       <c r="J66" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="67" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" ht="17.25" customHeight="1">
       <c r="A67" t="s">
         <v>9</v>
       </c>
       <c r="B67" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C67" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D67" s="3">
         <v>64</v>
       </c>
       <c r="E67" t="s">
+        <v>89</v>
+      </c>
+      <c r="F67" s="7">
+        <v>0</v>
+      </c>
+      <c r="G67" s="7">
+        <v>0</v>
+      </c>
+      <c r="H67" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I67" t="s">
         <v>90</v>
       </c>
-      <c r="F67" s="7">
-        <v>0</v>
-      </c>
-      <c r="G67" s="7">
-        <v>0</v>
-      </c>
-      <c r="H67" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I67" t="s">
-        <v>91</v>
-      </c>
       <c r="J67" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="68" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" ht="17.25" customHeight="1">
       <c r="A68" t="s">
         <v>9</v>
       </c>
       <c r="B68" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C68" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D68" s="3">
         <v>65</v>
       </c>
       <c r="E68" t="s">
+        <v>91</v>
+      </c>
+      <c r="F68" s="7">
+        <v>0</v>
+      </c>
+      <c r="G68" s="7">
+        <v>0</v>
+      </c>
+      <c r="H68" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I68" t="s">
         <v>92</v>
       </c>
-      <c r="F68" s="7">
-        <v>0</v>
-      </c>
-      <c r="G68" s="7">
-        <v>0</v>
-      </c>
-      <c r="H68" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I68" t="s">
-        <v>93</v>
-      </c>
       <c r="J68" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="69" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" ht="17.25" customHeight="1">
       <c r="A69" t="s">
         <v>9</v>
       </c>
       <c r="B69" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C69" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D69" s="3">
         <v>66</v>
       </c>
       <c r="E69" t="s">
+        <v>93</v>
+      </c>
+      <c r="F69" s="7">
+        <v>0</v>
+      </c>
+      <c r="G69" s="7">
+        <v>0</v>
+      </c>
+      <c r="H69" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I69" t="s">
         <v>94</v>
       </c>
-      <c r="F69" s="7">
-        <v>0</v>
-      </c>
-      <c r="G69" s="7">
-        <v>0</v>
-      </c>
-      <c r="H69" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I69" t="s">
-        <v>95</v>
-      </c>
       <c r="J69" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="70" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" ht="17.25" customHeight="1">
       <c r="A70" t="s">
         <v>9</v>
       </c>
       <c r="B70" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C70" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D70" s="3">
         <v>67</v>
       </c>
       <c r="E70" t="s">
+        <v>95</v>
+      </c>
+      <c r="F70" s="7">
+        <v>0</v>
+      </c>
+      <c r="G70" s="7">
+        <v>0</v>
+      </c>
+      <c r="H70" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I70" t="s">
         <v>96</v>
       </c>
-      <c r="F70" s="7">
-        <v>0</v>
-      </c>
-      <c r="G70" s="7">
-        <v>0</v>
-      </c>
-      <c r="H70" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I70" t="s">
-        <v>97</v>
-      </c>
       <c r="J70" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="71" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" ht="17.25" customHeight="1">
       <c r="A71" t="s">
         <v>9</v>
       </c>
       <c r="B71" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C71" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D71" s="3">
         <v>68</v>
       </c>
       <c r="E71" t="s">
+        <v>97</v>
+      </c>
+      <c r="F71" s="7">
+        <v>0</v>
+      </c>
+      <c r="G71" s="7">
+        <v>0</v>
+      </c>
+      <c r="H71" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I71" t="s">
         <v>98</v>
       </c>
-      <c r="F71" s="7">
-        <v>0</v>
-      </c>
-      <c r="G71" s="7">
-        <v>0</v>
-      </c>
-      <c r="H71" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I71" t="s">
-        <v>99</v>
-      </c>
       <c r="J71" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="72" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" ht="17.25" customHeight="1">
       <c r="A72" t="s">
         <v>9</v>
       </c>
       <c r="B72" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C72" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D72" s="3">
         <v>69</v>
       </c>
       <c r="E72" t="s">
+        <v>99</v>
+      </c>
+      <c r="F72" s="7">
+        <v>0</v>
+      </c>
+      <c r="G72" s="7">
+        <v>0</v>
+      </c>
+      <c r="H72" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I72" t="s">
         <v>100</v>
       </c>
-      <c r="F72" s="7">
-        <v>0</v>
-      </c>
-      <c r="G72" s="7">
-        <v>0</v>
-      </c>
-      <c r="H72" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I72" t="s">
-        <v>101</v>
-      </c>
       <c r="J72" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="73" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10" ht="17.25" customHeight="1">
       <c r="A73" t="s">
         <v>9</v>
       </c>
       <c r="B73" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C73" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D73" s="3">
         <v>70</v>
       </c>
       <c r="E73" t="s">
+        <v>101</v>
+      </c>
+      <c r="F73" s="7">
+        <v>0</v>
+      </c>
+      <c r="G73" s="7">
+        <v>0</v>
+      </c>
+      <c r="H73" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I73" t="s">
         <v>102</v>
       </c>
-      <c r="F73" s="7">
-        <v>0</v>
-      </c>
-      <c r="G73" s="7">
-        <v>0</v>
-      </c>
-      <c r="H73" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I73" t="s">
-        <v>103</v>
-      </c>
       <c r="J73" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="74" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" ht="17.25" customHeight="1">
       <c r="A74" t="s">
         <v>9</v>
       </c>
       <c r="B74" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C74" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D74" s="3">
         <v>71</v>
       </c>
       <c r="E74" t="s">
+        <v>103</v>
+      </c>
+      <c r="F74" s="7">
+        <v>0</v>
+      </c>
+      <c r="G74" s="7">
+        <v>0</v>
+      </c>
+      <c r="H74" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I74" t="s">
         <v>104</v>
       </c>
-      <c r="F74" s="7">
-        <v>0</v>
-      </c>
-      <c r="G74" s="7">
-        <v>0</v>
-      </c>
-      <c r="H74" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I74" t="s">
-        <v>105</v>
-      </c>
       <c r="J74" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="75" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" ht="17.25" customHeight="1">
       <c r="A75" t="s">
         <v>9</v>
       </c>
       <c r="B75" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C75" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D75" s="3">
         <v>72</v>
       </c>
       <c r="E75" t="s">
+        <v>105</v>
+      </c>
+      <c r="F75" s="7">
+        <v>0</v>
+      </c>
+      <c r="G75" s="7">
+        <v>0</v>
+      </c>
+      <c r="H75" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I75" t="s">
         <v>106</v>
       </c>
-      <c r="F75" s="7">
-        <v>0</v>
-      </c>
-      <c r="G75" s="7">
-        <v>0</v>
-      </c>
-      <c r="H75" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I75" t="s">
-        <v>107</v>
-      </c>
       <c r="J75" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="76" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" ht="17.25" customHeight="1">
       <c r="A76" t="s">
         <v>9</v>
       </c>
       <c r="B76" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C76" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D76" s="3">
         <v>73</v>
       </c>
       <c r="E76" t="s">
+        <v>107</v>
+      </c>
+      <c r="F76" s="7">
+        <v>0</v>
+      </c>
+      <c r="G76" s="7">
+        <v>0</v>
+      </c>
+      <c r="H76" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I76" t="s">
         <v>108</v>
       </c>
-      <c r="F76" s="7">
-        <v>0</v>
-      </c>
-      <c r="G76" s="7">
-        <v>0</v>
-      </c>
-      <c r="H76" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I76" t="s">
-        <v>109</v>
-      </c>
       <c r="J76" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="77" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10" ht="17.25" customHeight="1">
       <c r="A77" t="s">
         <v>9</v>
       </c>
       <c r="B77" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C77" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D77" s="3">
         <v>74</v>
       </c>
       <c r="E77" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" s="7">
+        <v>0</v>
+      </c>
+      <c r="G77" s="7">
+        <v>0</v>
+      </c>
+      <c r="H77" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I77" t="s">
         <v>110</v>
       </c>
-      <c r="F77" s="7">
-        <v>0</v>
-      </c>
-      <c r="G77" s="7">
-        <v>0</v>
-      </c>
-      <c r="H77" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I77" t="s">
-        <v>111</v>
-      </c>
       <c r="J77" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="78" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10" ht="17.25" customHeight="1">
       <c r="A78" t="s">
         <v>9</v>
       </c>
       <c r="B78" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C78" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D78" s="3">
         <v>75</v>
       </c>
       <c r="E78" t="s">
+        <v>111</v>
+      </c>
+      <c r="F78" s="7">
+        <v>0</v>
+      </c>
+      <c r="G78" s="7">
+        <v>0</v>
+      </c>
+      <c r="H78" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I78" t="s">
         <v>112</v>
       </c>
-      <c r="F78" s="7">
-        <v>0</v>
-      </c>
-      <c r="G78" s="7">
-        <v>0</v>
-      </c>
-      <c r="H78" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I78" t="s">
-        <v>113</v>
-      </c>
       <c r="J78" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="79" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" ht="17.25" customHeight="1">
       <c r="A79" t="s">
         <v>9</v>
       </c>
       <c r="B79" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C79" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D79" s="3">
         <v>76</v>
       </c>
       <c r="E79" t="s">
+        <v>113</v>
+      </c>
+      <c r="F79" s="7">
+        <v>0</v>
+      </c>
+      <c r="G79" s="7">
+        <v>0</v>
+      </c>
+      <c r="H79" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I79" t="s">
         <v>114</v>
       </c>
-      <c r="F79" s="7">
-        <v>0</v>
-      </c>
-      <c r="G79" s="7">
-        <v>0</v>
-      </c>
-      <c r="H79" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I79" t="s">
-        <v>115</v>
-      </c>
       <c r="J79" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="80" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" ht="17.25" customHeight="1">
       <c r="A80" t="s">
         <v>9</v>
       </c>
       <c r="B80" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C80" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D80" s="3">
         <v>77</v>
       </c>
       <c r="E80" t="s">
+        <v>115</v>
+      </c>
+      <c r="F80" s="7">
+        <v>0</v>
+      </c>
+      <c r="G80" s="7">
+        <v>0</v>
+      </c>
+      <c r="H80" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I80" t="s">
         <v>116</v>
       </c>
-      <c r="F80" s="7">
-        <v>0</v>
-      </c>
-      <c r="G80" s="7">
-        <v>0</v>
-      </c>
-      <c r="H80" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I80" t="s">
-        <v>117</v>
-      </c>
       <c r="J80" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="81" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" ht="17.25" customHeight="1">
       <c r="A81" t="s">
         <v>9</v>
       </c>
       <c r="B81" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C81" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D81" s="3">
         <v>78</v>
       </c>
       <c r="E81" t="s">
+        <v>117</v>
+      </c>
+      <c r="F81" s="7">
+        <v>0</v>
+      </c>
+      <c r="G81" s="7">
+        <v>0</v>
+      </c>
+      <c r="H81" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I81" t="s">
         <v>118</v>
       </c>
-      <c r="F81" s="7">
-        <v>0</v>
-      </c>
-      <c r="G81" s="7">
-        <v>0</v>
-      </c>
-      <c r="H81" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I81" t="s">
-        <v>119</v>
-      </c>
       <c r="J81" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="82" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" ht="17.25" customHeight="1">
       <c r="A82" t="s">
         <v>9</v>
       </c>
       <c r="B82" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C82" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D82" s="3">
         <v>79</v>
       </c>
       <c r="E82" t="s">
+        <v>119</v>
+      </c>
+      <c r="F82" s="7">
+        <v>0</v>
+      </c>
+      <c r="G82" s="7">
+        <v>0</v>
+      </c>
+      <c r="H82" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I82" t="s">
         <v>120</v>
       </c>
-      <c r="F82" s="7">
-        <v>0</v>
-      </c>
-      <c r="G82" s="7">
-        <v>0</v>
-      </c>
-      <c r="H82" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I82" t="s">
-        <v>121</v>
-      </c>
       <c r="J82" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="83" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" ht="17.25" customHeight="1">
       <c r="A83" t="s">
         <v>9</v>
       </c>
       <c r="B83" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C83" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D83" s="3">
         <v>80</v>
       </c>
       <c r="E83" t="s">
+        <v>121</v>
+      </c>
+      <c r="F83" s="7">
+        <v>0</v>
+      </c>
+      <c r="G83" s="7">
+        <v>0</v>
+      </c>
+      <c r="H83" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I83" t="s">
         <v>122</v>
       </c>
-      <c r="F83" s="7">
-        <v>0</v>
-      </c>
-      <c r="G83" s="7">
-        <v>0</v>
-      </c>
-      <c r="H83" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I83" t="s">
-        <v>123</v>
-      </c>
       <c r="J83" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="84" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" ht="17.25" customHeight="1">
       <c r="A84" t="s">
         <v>9</v>
       </c>
       <c r="B84" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C84" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D84" s="3">
         <v>81</v>
       </c>
       <c r="E84" t="s">
+        <v>123</v>
+      </c>
+      <c r="F84" s="7">
+        <v>0</v>
+      </c>
+      <c r="G84" s="7">
+        <v>0</v>
+      </c>
+      <c r="H84" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I84" t="s">
         <v>124</v>
       </c>
-      <c r="F84" s="7">
-        <v>0</v>
-      </c>
-      <c r="G84" s="7">
-        <v>0</v>
-      </c>
-      <c r="H84" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I84" t="s">
-        <v>125</v>
-      </c>
       <c r="J84" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="85" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" ht="17.25" customHeight="1">
       <c r="A85" t="s">
         <v>9</v>
       </c>
       <c r="B85" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C85" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D85" s="3">
         <v>82</v>
       </c>
       <c r="E85" t="s">
+        <v>125</v>
+      </c>
+      <c r="F85" s="7">
+        <v>0</v>
+      </c>
+      <c r="G85" s="7">
+        <v>0</v>
+      </c>
+      <c r="H85" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I85" t="s">
         <v>126</v>
       </c>
-      <c r="F85" s="7">
-        <v>0</v>
-      </c>
-      <c r="G85" s="7">
-        <v>0</v>
-      </c>
-      <c r="H85" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I85" t="s">
-        <v>127</v>
-      </c>
       <c r="J85" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="86" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" ht="17.25" customHeight="1">
       <c r="A86" t="s">
         <v>9</v>
       </c>
       <c r="B86" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C86" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D86" s="3">
         <v>83</v>
       </c>
       <c r="E86" t="s">
+        <v>127</v>
+      </c>
+      <c r="F86" s="7">
+        <v>0</v>
+      </c>
+      <c r="G86" s="7">
+        <v>0</v>
+      </c>
+      <c r="H86" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I86" t="s">
         <v>128</v>
       </c>
-      <c r="F86" s="7">
-        <v>0</v>
-      </c>
-      <c r="G86" s="7">
-        <v>0</v>
-      </c>
-      <c r="H86" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I86" t="s">
-        <v>129</v>
-      </c>
       <c r="J86" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="87" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" ht="17.25" customHeight="1">
       <c r="A87" t="s">
         <v>9</v>
       </c>
       <c r="B87" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C87" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D87" s="3">
         <v>84</v>
       </c>
       <c r="E87" t="s">
+        <v>129</v>
+      </c>
+      <c r="F87" s="7">
+        <v>0</v>
+      </c>
+      <c r="G87" s="7">
+        <v>0</v>
+      </c>
+      <c r="H87" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I87" t="s">
         <v>130</v>
       </c>
-      <c r="F87" s="7">
-        <v>0</v>
-      </c>
-      <c r="G87" s="7">
-        <v>0</v>
-      </c>
-      <c r="H87" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I87" t="s">
-        <v>131</v>
-      </c>
       <c r="J87" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="88" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" ht="17.25" customHeight="1">
       <c r="A88" t="s">
         <v>9</v>
       </c>
       <c r="B88" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C88" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D88" s="3">
         <v>85</v>
       </c>
       <c r="E88" t="s">
+        <v>131</v>
+      </c>
+      <c r="F88" s="7">
+        <v>0</v>
+      </c>
+      <c r="G88" s="7">
+        <v>0</v>
+      </c>
+      <c r="H88" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I88" t="s">
         <v>132</v>
       </c>
-      <c r="F88" s="7">
-        <v>0</v>
-      </c>
-      <c r="G88" s="7">
-        <v>0</v>
-      </c>
-      <c r="H88" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I88" t="s">
-        <v>133</v>
-      </c>
       <c r="J88" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="89" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" ht="17.25" customHeight="1">
       <c r="A89" t="s">
         <v>9</v>
       </c>
       <c r="B89" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C89" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D89" s="3">
         <v>86</v>
       </c>
       <c r="E89" t="s">
+        <v>133</v>
+      </c>
+      <c r="F89" s="7">
+        <v>0</v>
+      </c>
+      <c r="G89" s="7">
+        <v>0</v>
+      </c>
+      <c r="H89" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I89" t="s">
         <v>134</v>
       </c>
-      <c r="F89" s="7">
-        <v>0</v>
-      </c>
-      <c r="G89" s="7">
-        <v>0</v>
-      </c>
-      <c r="H89" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I89" t="s">
-        <v>135</v>
-      </c>
       <c r="J89" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="90" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" ht="17.25" customHeight="1">
       <c r="A90" t="s">
         <v>9</v>
       </c>
       <c r="B90" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C90" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D90" s="3">
         <v>87</v>
       </c>
       <c r="E90" t="s">
+        <v>135</v>
+      </c>
+      <c r="F90" s="7">
+        <v>0</v>
+      </c>
+      <c r="G90" s="7">
+        <v>0</v>
+      </c>
+      <c r="H90" s="5">
+        <v>2018</v>
+      </c>
+      <c r="I90" t="s">
         <v>136</v>
       </c>
-      <c r="F90" s="7">
-        <v>0</v>
-      </c>
-      <c r="G90" s="7">
-        <v>0</v>
-      </c>
-      <c r="H90" s="5">
-        <v>2018</v>
-      </c>
-      <c r="I90" t="s">
-        <v>137</v>
-      </c>
       <c r="J90" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="91" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4121,16 +4118,16 @@
         <v>9</v>
       </c>
       <c r="B91" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C91" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D91" s="3">
         <v>88</v>
       </c>
       <c r="E91" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="F91" s="7">
         <v>99.5</v>
@@ -4142,10 +4139,10 @@
         <v>2012</v>
       </c>
       <c r="I91" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="J91" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="92" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4153,16 +4150,16 @@
         <v>9</v>
       </c>
       <c r="B92" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C92" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D92" s="3">
         <v>89</v>
       </c>
       <c r="E92" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="F92" s="7">
         <v>200</v>
@@ -4174,10 +4171,10 @@
         <v>2017</v>
       </c>
       <c r="I92" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J92" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="93" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4185,16 +4182,16 @@
         <v>9</v>
       </c>
       <c r="B93" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C93" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D93" s="3">
         <v>90</v>
       </c>
       <c r="E93" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F93" s="7">
         <v>0</v>
@@ -4206,10 +4203,10 @@
         <v>2017</v>
       </c>
       <c r="I93" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="J93" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="94" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4217,16 +4214,16 @@
         <v>9</v>
       </c>
       <c r="B94" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C94" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D94" s="3">
         <v>91</v>
       </c>
       <c r="E94" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F94" s="7">
         <v>0</v>
@@ -4238,10 +4235,10 @@
         <v>2017</v>
       </c>
       <c r="I94" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="J94" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="95" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4249,16 +4246,16 @@
         <v>9</v>
       </c>
       <c r="B95" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C95" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D95" s="3">
         <v>92</v>
       </c>
       <c r="E95" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F95" s="7">
         <v>0</v>
@@ -4270,10 +4267,10 @@
         <v>2017</v>
       </c>
       <c r="I95" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="J95" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="96" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4281,16 +4278,16 @@
         <v>9</v>
       </c>
       <c r="B96" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C96" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D96" s="3">
         <v>93</v>
       </c>
       <c r="E96" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="F96" s="7">
         <v>0</v>
@@ -4302,10 +4299,10 @@
         <v>2017</v>
       </c>
       <c r="I96" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="J96" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="97" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4313,16 +4310,16 @@
         <v>9</v>
       </c>
       <c r="B97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C97" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D97" s="3">
         <v>94</v>
       </c>
       <c r="E97" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F97" s="7">
         <v>0</v>
@@ -4334,10 +4331,10 @@
         <v>2017</v>
       </c>
       <c r="I97" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="J97" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="98" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4345,16 +4342,16 @@
         <v>9</v>
       </c>
       <c r="B98" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C98" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D98" s="3">
         <v>95</v>
       </c>
       <c r="E98" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F98" s="7">
         <v>0</v>
@@ -4366,10 +4363,10 @@
         <v>2017</v>
       </c>
       <c r="I98" t="s">
+        <v>187</v>
+      </c>
+      <c r="J98" t="s">
         <v>189</v>
-      </c>
-      <c r="J98" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="99" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4377,16 +4374,16 @@
         <v>9</v>
       </c>
       <c r="B99" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C99" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D99" s="3">
         <v>96</v>
       </c>
       <c r="E99" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="F99" s="7">
         <v>0</v>
@@ -4398,10 +4395,10 @@
         <v>2017</v>
       </c>
       <c r="I99" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J99" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="100" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4409,16 +4406,16 @@
         <v>9</v>
       </c>
       <c r="B100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C100" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D100" s="3">
         <v>97</v>
       </c>
       <c r="E100" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="F100" s="7">
         <v>0</v>
@@ -4430,10 +4427,10 @@
         <v>2017</v>
       </c>
       <c r="I100" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="J100" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="101" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4441,16 +4438,16 @@
         <v>9</v>
       </c>
       <c r="B101" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C101" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D101" s="3">
         <v>98</v>
       </c>
       <c r="E101" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="F101" s="7">
         <v>0</v>
@@ -4462,10 +4459,10 @@
         <v>2017</v>
       </c>
       <c r="I101" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="J101" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="102" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4473,16 +4470,16 @@
         <v>9</v>
       </c>
       <c r="B102" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C102" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D102" s="3">
         <v>99</v>
       </c>
       <c r="E102" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F102" s="7">
         <v>0</v>
@@ -4494,10 +4491,10 @@
         <v>2017</v>
       </c>
       <c r="I102" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J102" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="103" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4505,16 +4502,16 @@
         <v>9</v>
       </c>
       <c r="B103" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C103" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D103" s="3">
         <v>100</v>
       </c>
       <c r="E103" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F103" s="7">
         <v>40</v>
@@ -4526,10 +4523,10 @@
         <v>2017</v>
       </c>
       <c r="I103" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="J103" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="104" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4537,16 +4534,16 @@
         <v>9</v>
       </c>
       <c r="B104" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C104" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D104" s="3">
         <v>101</v>
       </c>
       <c r="E104" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F104" s="7">
         <v>40</v>
@@ -4558,10 +4555,10 @@
         <v>2016</v>
       </c>
       <c r="I104" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="J104" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="105" spans="1:10" ht="19.5" hidden="1" customHeight="1">
@@ -4569,16 +4566,16 @@
         <v>9</v>
       </c>
       <c r="B105" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C105" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D105" s="3">
         <v>102</v>
       </c>
       <c r="E105" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F105" s="7">
         <v>40</v>
@@ -4590,10 +4587,10 @@
         <v>2016</v>
       </c>
       <c r="I105" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J105" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
     </row>
     <row r="106" spans="1:10" ht="17.25" hidden="1" customHeight="1">
@@ -4601,16 +4598,16 @@
         <v>9</v>
       </c>
       <c r="B106" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C106" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D106" s="3">
         <v>105</v>
       </c>
       <c r="E106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="F106" s="7">
         <v>213.4</v>
@@ -4622,10 +4619,10 @@
         <v>2018</v>
       </c>
       <c r="I106" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="J106" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="107" spans="1:10" ht="17.25" hidden="1" customHeight="1">
@@ -4633,16 +4630,16 @@
         <v>9</v>
       </c>
       <c r="B107" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C107" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D107" s="3">
         <v>106</v>
       </c>
       <c r="E107" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="F107" s="7">
         <v>107</v>
@@ -4654,10 +4651,10 @@
         <v>2018</v>
       </c>
       <c r="I107" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="J107" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="108" spans="1:10" ht="17.25" hidden="1" customHeight="1">
@@ -4665,16 +4662,16 @@
         <v>9</v>
       </c>
       <c r="B108" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C108" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D108" s="3">
         <v>107</v>
       </c>
       <c r="E108" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="F108" s="7">
         <v>120.9</v>
@@ -4686,10 +4683,10 @@
         <v>2018</v>
       </c>
       <c r="I108" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="J108" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="109" spans="1:10" ht="17.25" hidden="1" customHeight="1">
@@ -4697,16 +4694,16 @@
         <v>9</v>
       </c>
       <c r="B109" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C109" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D109" s="3">
         <v>108</v>
       </c>
       <c r="E109" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="F109" s="7">
         <v>142.19999999999999</v>
@@ -4718,10 +4715,10 @@
         <v>2018</v>
       </c>
       <c r="I109" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="J109" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
     </row>
     <row r="110" spans="1:10" ht="17.25" hidden="1" customHeight="1">
@@ -4729,16 +4726,16 @@
         <v>9</v>
       </c>
       <c r="B110" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C110" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="D110" s="3">
         <v>109</v>
       </c>
       <c r="E110" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F110" s="7">
         <v>120.9</v>
@@ -4750,27 +4747,27 @@
         <v>2018</v>
       </c>
       <c r="I110" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="J110" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="111" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="111" spans="1:10" ht="17.25" customHeight="1">
       <c r="A111" t="s">
         <v>9</v>
       </c>
       <c r="B111" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C111" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D111" s="3">
         <v>110</v>
       </c>
       <c r="E111" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="F111" s="7">
         <v>50</v>
@@ -4782,27 +4779,27 @@
         <v>2017</v>
       </c>
       <c r="I111" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="J111" t="s">
-        <v>245</v>
-      </c>
-    </row>
-    <row r="112" spans="1:10" ht="17.25" hidden="1" customHeight="1">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="112" spans="1:10" ht="17.25" customHeight="1">
       <c r="A112" t="s">
         <v>9</v>
       </c>
       <c r="B112" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="C112" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D112" s="3">
         <v>111</v>
       </c>
       <c r="E112" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="F112" s="7">
         <v>65</v>
@@ -4814,10 +4811,10 @@
         <v>2021</v>
       </c>
       <c r="I112" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="J112" t="s">
-        <v>245</v>
+        <v>243</v>
       </c>
     </row>
     <row r="113" spans="4:8" ht="17.25" customHeight="1">
@@ -4920,7 +4917,7 @@
   <autoFilter ref="A1:J112" xr:uid="{00000000-0001-0000-0000-000000000000}">
     <filterColumn colId="1">
       <filters>
-        <filter val="Patina"/>
+        <filter val="Ottchil (Korean Lacquer Work)"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>